<commit_message>
Updated to reflect testing.
</commit_message>
<xml_diff>
--- a/TestLogs/pipeline example data testing assignment.xlsx
+++ b/TestLogs/pipeline example data testing assignment.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11205"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>dave</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>ex. data used</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>err file contains what you expect in the .out file</t>
+  </si>
+  <si>
+    <t>dongwang/alphasim_1</t>
   </si>
 </sst>
 </file>
@@ -448,13 +457,13 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="5" max="5" width="66" customWidth="1"/>
   </cols>
   <sheetData>
@@ -482,6 +491,15 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Updated to reflect current progress
</commit_message>
<xml_diff>
--- a/TestLogs/pipeline example data testing assignment.xlsx
+++ b/TestLogs/pipeline example data testing assignment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19220" yWindow="440" windowWidth="19180" windowHeight="22520" xr2:uid="{C9D4A7A6-BA46-454A-BCFB-290FA19DD55C}"/>
+    <workbookView xWindow="19200" yWindow="440" windowWidth="19200" windowHeight="22540" xr2:uid="{C9D4A7A6-BA46-454A-BCFB-290FA19DD55C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>dave</t>
   </si>
@@ -86,7 +86,22 @@
     <t>err file contains what you expect in the .out file</t>
   </si>
   <si>
-    <t>dongwang/alphasim_1</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>not available in apps-list for Agave apps</t>
+  </si>
+  <si>
+    <t>dongwang/</t>
+  </si>
+  <si>
+    <t>version 2 is not public, working on getting published</t>
+  </si>
+  <si>
+    <t>Might be a problem with not being public, might be a problem with not sourcing dir correclty</t>
+  </si>
+  <si>
+    <t>Plink</t>
   </si>
 </sst>
 </file>
@@ -457,14 +472,14 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="66" customWidth="1"/>
+    <col min="5" max="5" width="79.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -492,7 +507,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -508,13 +523,25 @@
       <c r="B3" t="s">
         <v>0</v>
       </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -563,6 +590,15 @@
       </c>
       <c r="B11" t="s">
         <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>